<commit_message>
More Bugfixes and test/doc improvements: 1) Version string > 16 characters returning a 500 error \n 2)Access Service version of a deleted Service 3) Some test and documentation updates and improvements
</commit_message>
<xml_diff>
--- a/BugReport.xlsx
+++ b/BugReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suryarekha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\kongtakehome\kong-takehometask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBB195E-7A27-443E-941B-8A1528A4D5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD49818-D6C2-4933-B4E0-E7309F36C3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{72C219AB-2C96-4BEA-88A3-D3840232E7F1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{72C219AB-2C96-4BEA-88A3-D3840232E7F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>S.No</t>
   </si>
@@ -354,6 +354,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Should this be a 404</t>
+  </si>
+  <si>
+    <t>Deleted Service doesn’t affect the linked Service version</t>
+  </si>
+  <si>
+    <t>API under test: DELETE  /v1/services/{svcId}
+Steps to reproduce: 
+1. Create a Service and the service version
+2. List the service version and see the service version fecthed successfully
+3. Delete the service
+See that the deleted service has no impct on the linked service versions</t>
+  </si>
+  <si>
+    <t>Delete Service
+Question/Clarification</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -414,15 +429,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -759,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35D771E-7B7E-472F-8446-B0EB3CF8603D}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -988,6 +1018,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>